<commit_message>
Count the total number of violations IN Spark.py
</commit_message>
<xml_diff>
--- a/Data/New data.xlsx
+++ b/Data/New data.xlsx
@@ -3374,7 +3374,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D562"/>
+  <dimension ref="A1:D570"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14640,6 +14640,166 @@
         <v>6.9</v>
       </c>
     </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>18_Car-CA</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Cairo</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>Giza</t>
+        </is>
+      </c>
+      <c r="D563" t="n">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>18_Car-GIZ</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Giza</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>Qalyubia</t>
+        </is>
+      </c>
+      <c r="D564" t="n">
+        <v>31.8</v>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>180_Car-CA</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Cairo</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>Giza</t>
+        </is>
+      </c>
+      <c r="D565" t="n">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>180_Car-GIZ</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Giza</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>Qalyubia</t>
+        </is>
+      </c>
+      <c r="D566" t="n">
+        <v>31.8</v>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>181_Car-CA</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Cairo</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>Giza</t>
+        </is>
+      </c>
+      <c r="D567" t="n">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>181_Car-GIZ</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Giza</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>Qalyubia</t>
+        </is>
+      </c>
+      <c r="D568" t="n">
+        <v>31.8</v>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>123456_Car-CA</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Cairo</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>Giza</t>
+        </is>
+      </c>
+      <c r="D569" t="n">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>123456_Car-GIZ</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Giza</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>Qalyubia</t>
+        </is>
+      </c>
+      <c r="D570" t="n">
+        <v>31.8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>